<commit_message>
update player active view.
</commit_message>
<xml_diff>
--- a/api_service/public/download/会员账号批量导入模板.xlsx
+++ b/api_service/public/download/会员账号批量导入模板.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dongchen/WebstormProjects/active_center/api_service/public/download/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08AA3F90-5F39-2D44-8F08-1B0B30D948BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0837AD-9431-5B4B-8C65-03EAF2CF8574}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2440" yWindow="460" windowWidth="25600" windowHeight="14900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -522,7 +522,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
增加leader house_code 属性维护 (#21)
</commit_message>
<xml_diff>
--- a/api_service/public/download/会员账号批量导入模板.xlsx
+++ b/api_service/public/download/会员账号批量导入模板.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dongchen/WebstormProjects/active_center/api_service/public/download/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0837AD-9431-5B4B-8C65-03EAF2CF8574}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB64929-B152-1746-A3BB-22A8131193AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2440" yWindow="460" windowWidth="25600" windowHeight="14900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>手机号</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -42,6 +42,14 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>备注</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>鸽棚号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -50,7 +58,7 @@
         <rFont val="等线 (正文)"/>
         <charset val="134"/>
       </rPr>
-      <t>角色和手机号为必填项，其余3项可选项。</t>
+      <t>角色和手机号为必填项，角色为团长时，鸽棚号也是必填项。其余项目可选项。</t>
     </r>
     <r>
       <rPr>
@@ -78,10 +86,6 @@
       </rPr>
       <t>登录系统实际使用账号和密码登录</t>
     </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>备注</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -519,19 +523,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="4" width="15" customWidth="1"/>
-    <col min="6" max="6" width="13.83203125" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16">
+    <row r="1" spans="1:13" ht="16">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -550,171 +554,174 @@
       <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="F2" s="4"/>
-      <c r="G2" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="6"/>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="G2" s="4"/>
+      <c r="H2" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="F3" s="4"/>
-      <c r="G3" s="6"/>
+      <c r="M2" s="6"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="G3" s="4"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="F4" s="4"/>
-      <c r="G4" s="6"/>
+      <c r="M3" s="6"/>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="G4" s="4"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
-    </row>
-    <row r="5" spans="1:12" ht="16">
+      <c r="M4" s="6"/>
+    </row>
+    <row r="5" spans="1:13" ht="16">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="6"/>
+      <c r="G5" s="4"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="G6" s="6"/>
+      <c r="M5" s="6"/>
+    </row>
+    <row r="6" spans="1:13">
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="G7" s="6"/>
+      <c r="M6" s="6"/>
+    </row>
+    <row r="7" spans="1:13">
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="G8" s="6"/>
+      <c r="M7" s="6"/>
+    </row>
+    <row r="8" spans="1:13">
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="G9" s="6"/>
+      <c r="M8" s="6"/>
+    </row>
+    <row r="9" spans="1:13">
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="G10" s="6"/>
+      <c r="M9" s="6"/>
+    </row>
+    <row r="10" spans="1:13">
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="G11" s="6"/>
+      <c r="M10" s="6"/>
+    </row>
+    <row r="11" spans="1:13">
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="G12" s="6"/>
+      <c r="M11" s="6"/>
+    </row>
+    <row r="12" spans="1:13">
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="G13" s="6"/>
+      <c r="M12" s="6"/>
+    </row>
+    <row r="13" spans="1:13">
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="G14" s="6"/>
+      <c r="M13" s="6"/>
+    </row>
+    <row r="14" spans="1:13">
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="G15" s="6"/>
+      <c r="M14" s="6"/>
+    </row>
+    <row r="15" spans="1:13">
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="G16" s="6"/>
+      <c r="M15" s="6"/>
+    </row>
+    <row r="16" spans="1:13">
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
-    </row>
-    <row r="17" spans="7:12">
-      <c r="G17" s="6"/>
+      <c r="M16" s="6"/>
+    </row>
+    <row r="17" spans="8:13">
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
-    </row>
-    <row r="18" spans="7:12">
-      <c r="G18" s="6"/>
+      <c r="M17" s="6"/>
+    </row>
+    <row r="18" spans="8:13">
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
-    </row>
-    <row r="19" spans="7:12">
-      <c r="G19" s="6"/>
+      <c r="M18" s="6"/>
+    </row>
+    <row r="19" spans="8:13">
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
-    </row>
-    <row r="20" spans="7:12">
-      <c r="G20" s="6"/>
+      <c r="M19" s="6"/>
+    </row>
+    <row r="20" spans="8:13">
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="G2:L20"/>
+    <mergeCell ref="H2:M20"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="1">

</xml_diff>